<commit_message>
Update Author/Affiliations and Add Citation Checklist
</commit_message>
<xml_diff>
--- a/doc/authors_and_affiliations.xlsx
+++ b/doc/authors_and_affiliations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rachelhoffman/Documents/GitHub/15yrsChange/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6428F363-19C8-4043-89F0-168DDF64684A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{443A4368-FFA0-7F45-A167-B651A0919966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16260" xr2:uid="{289D093C-E529-D74F-A7E5-7EAA1B7B8D4E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14280" windowHeight="18000" xr2:uid="{289D093C-E529-D74F-A7E5-7EAA1B7B8D4E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
   <si>
     <t>Name</t>
   </si>
@@ -98,9 +98,6 @@
     <t>Cameron Dow</t>
   </si>
   <si>
-    <t>Department of Biology, West Virginia University, Morgantown, WV, 26506, USA</t>
-  </si>
-  <si>
     <t>Valentine Herrmann</t>
   </si>
   <si>
@@ -119,9 +116,6 @@
     <t>Lukas Magee</t>
   </si>
   <si>
-    <t>School of Forest, Fisheries, and Geomatics Sciences, University of Florida, Gainesville, Florida, 32603, USA</t>
-  </si>
-  <si>
     <t>mageel@ufl.edu</t>
   </si>
   <si>
@@ -156,7 +150,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Aptos Narrow (Body)"/>
       </rPr>
-      <t>1</t>
+      <t>2</t>
     </r>
     <r>
       <rPr>
@@ -166,7 +160,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Forest Global Earth Observatory, Smithsonian’s National Zoo &amp; Conservation Biology Institute, Front Royal, VA, 22630 USA</t>
+      <t>Forest Ecology Group, Smithsonian Environmental Research Center, Edgewater, MD 21037, USA</t>
     </r>
   </si>
   <si>
@@ -177,7 +171,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Aptos Narrow (Body)"/>
       </rPr>
-      <t>2</t>
+      <t>3</t>
     </r>
     <r>
       <rPr>
@@ -187,18 +181,65 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Forest Ecology Group, Smithsonian Environmental Research Center, Edgewater, MD 21037, USA</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
+      <t xml:space="preserve">Smithsonian Tropical Research Institute, Apartado, Balboa 0843-03092, Republica de Panamá  </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Forest Global Earth Observatory, Smithsonian Tropical Research Institute, Panama City, Panama </t>
+    </r>
+    <r>
+      <rPr>
         <sz val="12"/>
         <color rgb="FFFF0000"/>
         <rFont val="Aptos Narrow (Body)"/>
       </rPr>
       <t>3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Forest Global Earth Observatory, Smithsonian Environmental Research Center, Edgewater, MD 21037, United States of America </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Conservation Ecology Center, Smithsonian’s National Zoo &amp; Conservation Biology Institute, Front Royal, VA, 22630 USA </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <t>n_bourg@hotmail.com</t>
+  </si>
+  <si>
+    <t>Norman A. Bourg</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Conservation Ecology Center, Smithsonian’s National Zoo &amp; Conservation Biology Institute, Front Royal, VA </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>1</t>
     </r>
     <r>
       <rPr>
@@ -208,25 +249,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Smithsonian Tropical Research Institute, Apartado, Balboa 0843-03092, Republica de Panamá  </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Forest Global Earth Observatory, Smithsonian’s National Zoo &amp; Conservation Biology Institute, Front Royal, VA, 22630 USA </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow (Body)"/>
-      </rPr>
-      <t>1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Forest Global Earth Observatory, Smithsonian Tropical Research Institute, Panama City, Panama </t>
+      <t xml:space="preserve"> , 22630 USA; Forest Global Earth Observatory, Smithsonian Tropical Research Institute, Panama City, Panama </t>
     </r>
     <r>
       <rPr>
@@ -235,32 +258,6 @@
         <rFont val="Aptos Narrow (Body)"/>
       </rPr>
       <t>3</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Forest Global Earth Observatory, Smithsonian Environmental Research Center, Edgewater, MD 21037, United States of America </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow (Body)"/>
-      </rPr>
-      <t>2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Forest Global Earth Observatory, Smithsonian’s National Zoo &amp; Conservation Biology Institute, Front Royal, VA </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow (Body)"/>
-      </rPr>
-      <t>1</t>
     </r>
     <r>
       <rPr>
@@ -270,15 +267,20 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> , 22630 USA; Forest Global Earth Observatory, Smithsonian Tropical Research Institute, Panama City, Panama </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow (Body)"/>
-      </rPr>
-      <t>3</t>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Conservation Ecology Center, Smithsonian’s National Zoo &amp; Conservation Biology Institute, Front Royal, VA, 22630 USA </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>1</t>
     </r>
     <r>
       <rPr>
@@ -288,12 +290,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Forest Global Earth Observatory, Smithsonian’s National Zoo &amp; Conservation Biology Institute, Front Royal, VA, 22630 USA </t>
+      <t>; School of Forest, Fisheries, and Geomatics Sciences, University of Florida, Gainesville, Florida, 32603, USA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Conservation Ecology Center, Smithsonian’s National Zoo &amp; Conservation Biology Institute, Front Royal, VA, 22630 USA </t>
     </r>
     <r>
       <rPr>
@@ -311,15 +313,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> ; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow (Body)"/>
-      </rPr>
-      <t>Department of ______________</t>
+      <t>, Department of Biology, West Virginia University, Morgantown, WV, 26506, USA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t xml:space="preserve">1   </t>
     </r>
     <r>
       <rPr>
@@ -329,7 +334,48 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">, George Mason University, Fairfax, VA, 22030, USA  </t>
+      <t>Forest Global Earth Observatory, National Zoo &amp; Conservation Biology Institute, Front Royal, VA, 22630 USA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Conservation Ecology Center, Smithsonian’s National Zoo &amp; Conservation Biology Institute, Front Royal, VA, 22630 USA </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>Department of ______________,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> George Mason University, Fairfax, VA, 22030, USA  </t>
     </r>
   </si>
 </sst>
@@ -423,8 +469,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{01AD2269-EF6F-194F-A170-3FA8BC391899}" name="Table1" displayName="Table1" ref="A1:C16" totalsRowShown="0">
-  <autoFilter ref="A1:C16" xr:uid="{01AD2269-EF6F-194F-A170-3FA8BC391899}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{01AD2269-EF6F-194F-A170-3FA8BC391899}" name="Table1" displayName="Table1" ref="A1:C17" totalsRowShown="0">
+  <autoFilter ref="A1:C17" xr:uid="{01AD2269-EF6F-194F-A170-3FA8BC391899}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{1097122F-9FDC-2246-B096-BD1147652992}" name="Name"/>
     <tableColumn id="2" xr3:uid="{54E92C40-6511-7441-98DF-1E99BF9094C0}" name="Institutional Affliation" dataDxfId="0"/>
@@ -751,10 +797,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F9C0A7B-5B9E-DF4F-BADE-BD783972F1C1}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -780,7 +826,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -791,7 +837,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>11</v>
@@ -802,7 +848,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>13</v>
@@ -813,7 +859,7 @@
         <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>15</v>
@@ -824,7 +870,7 @@
         <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>17</v>
@@ -835,139 +881,150 @@
         <v>18</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="2" t="s">
+    </row>
+    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="B11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="17" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="2" t="s">
+      <c r="B17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C17" s="2"/>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C18" s="2"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="B20" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="B21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C16" r:id="rId1" display="teixeirak@si.edu" xr:uid="{11B3902E-67AF-AB4E-B573-0FC7BFED355A}"/>
+    <hyperlink ref="C17" r:id="rId1" display="teixeirak@si.edu" xr:uid="{11B3902E-67AF-AB4E-B573-0FC7BFED355A}"/>
     <hyperlink ref="C2" r:id="rId2" xr:uid="{53B15DCA-6F21-8C40-A563-53D8BF62BCB4}"/>
-    <hyperlink ref="C15" r:id="rId3" display="McSheaW@si.edu" xr:uid="{6583A198-E7E4-7543-B352-E7B2A4FA4D0F}"/>
+    <hyperlink ref="C16" r:id="rId3" display="McSheaW@si.edu" xr:uid="{6583A198-E7E4-7543-B352-E7B2A4FA4D0F}"/>
     <hyperlink ref="C3" r:id="rId4" xr:uid="{955DDCC8-8AD2-D14C-B3F3-A5495CD20854}"/>
     <hyperlink ref="C4" r:id="rId5" xr:uid="{EEDB88DD-BCF7-494E-9400-0A09ADB8331D}"/>
     <hyperlink ref="C5" r:id="rId6" xr:uid="{E7EDECF5-B80F-B943-B610-C48B8CDF1B36}"/>
@@ -980,10 +1037,11 @@
     <hyperlink ref="C12" r:id="rId13" xr:uid="{98769E43-C35C-6A4D-9727-AAF077F78FB8}"/>
     <hyperlink ref="C14" r:id="rId14" xr:uid="{D8B66242-E5D2-E544-A5A8-EE58E85377EA}"/>
     <hyperlink ref="C13" r:id="rId15" xr:uid="{59E07A76-9B28-B847-A10A-805C42619B94}"/>
+    <hyperlink ref="C15" r:id="rId16" xr:uid="{1A4D9F8D-25B9-CB4D-9CF4-508715A593C8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId16"/>
+    <tablePart r:id="rId17"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>